<commit_message>
fixed all mistakes and improved task 5
</commit_message>
<xml_diff>
--- a/Lesson_8/task_5.xlsx
+++ b/Lesson_8/task_5.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,42 +536,34 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>646-38-52</t>
+          <t>448-59-26</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>629-46-81</t>
+          <t>775-96-85</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>368-68-15</t>
+          <t>816-93-57</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>710-11-71</t>
+          <t>402-74-22</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>330-32-78</t>
+          <t>976-19-75</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>723-30-85</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
+          <t>528-96-42</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>